<commit_message>
After adding git links
</commit_message>
<xml_diff>
--- a/TrackingSheet.xlsx
+++ b/TrackingSheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmusham\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6D4D57-6EC3-48DD-A1B9-C36A7D4308A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aug 19" sheetId="1" r:id="rId1"/>
@@ -19,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -99,12 +94,18 @@
   </si>
   <si>
     <t xml:space="preserve">Watched Git videos </t>
+  </si>
+  <si>
+    <t>https://github.com/VarshaMusham/iTransformTracker.git</t>
+  </si>
+  <si>
+    <t>https://github.com/VarshaMusham/GitAssignment.git</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
@@ -757,11 +758,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -771,7 +772,7 @@
     <col min="5" max="5" width="13.1796875" customWidth="1"/>
     <col min="6" max="6" width="43.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.6328125" customWidth="1"/>
-    <col min="8" max="8" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.81640625" customWidth="1"/>
     <col min="9" max="9" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -842,7 +843,7 @@
       <c r="H4" s="22"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="11">
         <v>43690</v>
       </c>
@@ -857,10 +858,12 @@
         <v>22</v>
       </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="23"/>
+      <c r="H5" s="22" t="s">
+        <v>23</v>
+      </c>
       <c r="I5" s="10"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="11">
         <v>43691</v>
       </c>
@@ -875,7 +878,9 @@
         <v>21</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="23"/>
+      <c r="H6" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">

</xml_diff>